<commit_message>
HOMEACC-28: #comment update all Credit DB #time 3h 15m #description Design Database
</commit_message>
<xml_diff>
--- a/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/DB_Mapping.xlsx
+++ b/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/DB_Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minhphan/PycharmProjects/HomeAccounting/trial/MeoDemo_Final/Prepare_Manual/SpreadSheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miph272640\PycharmProjects\HomeAccounting\trial\MeoDemo_Final\Prepare_Manual\SpreadSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2DE82E-D3F1-5F41-AE89-03BEB725AFFE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC0F535-9952-480A-9B36-5ABD70AB2F1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36320" yWindow="4900" windowWidth="14000" windowHeight="15440" xr2:uid="{965CF788-C514-9342-AFBC-E7572D08F673}"/>
+    <workbookView xWindow="2520" yWindow="1530" windowWidth="21600" windowHeight="14490" xr2:uid="{965CF788-C514-9342-AFBC-E7572D08F673}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="62">
   <si>
     <t>Category</t>
   </si>
@@ -114,9 +113,6 @@
     <t>Income</t>
   </si>
   <si>
-    <t>In case manual adjustment</t>
-  </si>
-  <si>
     <t>Return</t>
   </si>
   <si>
@@ -217,28 +213,43 @@
   </si>
   <si>
     <t>Parent books, language lession, study materials</t>
+  </si>
+  <si>
+    <t>Out</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Manual Adjustment (not sure if needed)</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,6 +280,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -282,13 +299,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,18 +623,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFC7E0FB-6BD3-0542-B887-99EE566F6C80}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
     <col min="4" max="4" width="57.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -624,13 +642,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -638,13 +656,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -652,13 +670,13 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -666,13 +684,13 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -680,13 +698,13 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -694,13 +712,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -708,41 +726,41 @@
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -750,13 +768,13 @@
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -764,13 +782,13 @@
         <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
@@ -778,13 +796,13 @@
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -792,223 +810,225 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="C18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A19" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A21" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="C23" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="2" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="2" t="s">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="B28" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>34</v>
-      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>